<commit_message>
add three more unsupervised methods
</commit_message>
<xml_diff>
--- a/results/batch_effects/batch_effects_summarized_results.xlsx
+++ b/results/batch_effects/batch_effects_summarized_results.xlsx
@@ -9,13 +9,13 @@
     <sheet name="All" r:id="rId3" sheetId="1"/>
     <sheet name="Assigned" r:id="rId4" sheetId="2"/>
     <sheet name="Unassigned" r:id="rId5" sheetId="3"/>
-    <sheet name="Other metrics(unlabeled pctg, c" r:id="rId6" sheetId="4"/>
+    <sheet name="Supervised methods other metric" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="48">
   <si>
     <t>All results(assigned/unassigned combined)</t>
   </si>
@@ -149,16 +149,13 @@
     <t>Unassigned only</t>
   </si>
   <si>
-    <t>Other metrics(unlabeled pctg, cluster num...)</t>
+    <t>Other metrics(unlabeled pctg...)</t>
   </si>
   <si>
     <t>metrics</t>
   </si>
   <si>
     <t>unlabeled_pctg</t>
-  </si>
-  <si>
-    <t>cluster_num</t>
   </si>
   <si>
     <t>pred_type_max_pctg</t>
@@ -3474,25 +3471,25 @@
         <v>40</v>
       </c>
       <c r="E6" t="n">
-        <v>8.0</v>
+        <v>0.37656197230665317</v>
       </c>
       <c r="F6" t="n">
-        <v>6.0</v>
+        <v>0.3951367781155015</v>
       </c>
       <c r="G6" t="n">
-        <v>6.0</v>
+        <v>0.4998311381290105</v>
       </c>
       <c r="H6" t="n">
-        <v>6.0</v>
+        <v>0.4154002026342452</v>
       </c>
       <c r="I6" t="n">
-        <v>4.0</v>
+        <v>0.8831475852752448</v>
       </c>
       <c r="J6" t="n">
-        <v>6.0</v>
+        <v>0.7213779128672746</v>
       </c>
       <c r="K6" t="n">
-        <v>6.0</v>
+        <v>0.7112462006079028</v>
       </c>
       <c r="L6" t="n">
         <v>0.8920681447759645</v>
@@ -3569,22 +3566,22 @@
         <v>1.0</v>
       </c>
       <c r="F7" t="n">
-        <v>6.0</v>
+        <v>0.6700439040864573</v>
       </c>
       <c r="G7" t="n">
         <v>1.0</v>
       </c>
-      <c r="H7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1.0</v>
+      <c r="H7" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" t="e">
+        <v>#DIV/0!</v>
       </c>
       <c r="K7" t="n">
-        <v>6.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="L7" t="n">
         <v>0.7458019093026144</v>
@@ -3646,105 +3643,105 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
       </c>
       <c r="E8" t="n">
-        <v>0.37656197230665317</v>
+        <v>0.001962708537782139</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3951367781155015</v>
+        <v>0.7203140333660452</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4998311381290105</v>
+        <v>0.2237487733071639</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4154002026342452</v>
+        <v>0.02747791952894995</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8831475852752448</v>
+        <v>0.016683022571148183</v>
       </c>
       <c r="J8" t="n">
-        <v>0.7213779128672746</v>
+        <v>0.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.7112462006079028</v>
+        <v>0.0</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8920681447759645</v>
+        <v>0.5602951702053611</v>
       </c>
       <c r="M8" t="n">
-        <v>1.6408641369006336</v>
+        <v>1.613898679837703</v>
       </c>
       <c r="N8" t="n">
-        <v>0.07157846974079746</v>
+        <v>5.327317965954149</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0611139470251262</v>
+        <v>4.636286009871222</v>
       </c>
       <c r="P8" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4103177314656645</v>
+        <v>0.397796817625459</v>
       </c>
       <c r="R8" t="n">
-        <v>0.9658568741809688</v>
+        <v>0.7258413264338339</v>
       </c>
       <c r="S8" t="n">
-        <v>2927.0</v>
+        <v>1634.0</v>
       </c>
       <c r="T8" t="n">
-        <v>17631.0</v>
+        <v>18158.0</v>
       </c>
       <c r="U8" t="n">
-        <v>0.9459134290866236</v>
+        <v>0.16718577785086547</v>
       </c>
       <c r="V8" t="n">
-        <v>1.9791732004479081</v>
+        <v>1.550027473303311</v>
       </c>
       <c r="W8" t="n">
-        <v>0.07957574726334297</v>
+        <v>17.805182288798328</v>
       </c>
       <c r="X8" t="n">
-        <v>0.026827746582723605</v>
+        <v>24.355242868157283</v>
       </c>
       <c r="Y8" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.17662951705504898</v>
+        <v>0.43473994111874387</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.9662907227339798</v>
+        <v>0.6653024736202267</v>
       </c>
       <c r="AB8" t="n">
-        <v>2961.0</v>
+        <v>2038.0</v>
       </c>
       <c r="AC8" t="n">
-        <v>17631.0</v>
+        <v>18158.0</v>
       </c>
       <c r="AD8" t="n">
-        <v>735.447146316415</v>
+        <v>260186.17743712067</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
         <v>41</v>
@@ -3753,79 +3750,79 @@
         <v>1.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6700439040864573</v>
+        <v>0.04072620215897939</v>
       </c>
       <c r="G9" t="n">
+        <v>0.9862610402355251</v>
+      </c>
+      <c r="H9" t="n">
         <v>1.0</v>
       </c>
-      <c r="H9" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" t="e">
-        <v>#DIV/0!</v>
+      <c r="I9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.6666666666666666</v>
+        <v>4.906771344455348E-4</v>
       </c>
       <c r="L9" t="n">
-        <v>0.7458019093026144</v>
+        <v>0.5622018786890313</v>
       </c>
       <c r="M9" t="n">
-        <v>1.6408641369006336</v>
+        <v>1.613898679837703</v>
       </c>
       <c r="N9" t="n">
-        <v>1.0000126604182638</v>
+        <v>1.0003422257720689</v>
       </c>
       <c r="O9" t="n">
-        <v>1.58025677900131E-4</v>
+        <v>6.017339481372286E-4</v>
       </c>
       <c r="P9" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.4103177314656645</v>
+        <v>0.397796817625459</v>
       </c>
       <c r="R9" t="n">
         <v>0.0</v>
       </c>
       <c r="S9" t="n">
-        <v>2927.0</v>
+        <v>1634.0</v>
       </c>
       <c r="T9" t="n">
-        <v>8073.0</v>
+        <v>8755.0</v>
       </c>
       <c r="U9" t="n">
-        <v>0.7625564453272975</v>
+        <v>0.6023658796459858</v>
       </c>
       <c r="V9" t="n">
-        <v>1.9791732004479081</v>
+        <v>1.550027473303311</v>
       </c>
       <c r="W9" t="n">
-        <v>0.9999801670553027</v>
+        <v>1.0004491461137193</v>
       </c>
       <c r="X9" t="n">
-        <v>1.237001696619E-4</v>
+        <v>6.064841273867305E-4</v>
       </c>
       <c r="Y9" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.17662951705504898</v>
+        <v>0.43473994111874387</v>
       </c>
       <c r="AA9" t="n">
         <v>0.0</v>
       </c>
       <c r="AB9" t="n">
-        <v>2961.0</v>
+        <v>2038.0</v>
       </c>
       <c r="AC9" t="n">
-        <v>8073.0</v>
+        <v>8755.0</v>
       </c>
       <c r="AD9" t="n">
-        <v>2.0224697880663314</v>
+        <v>3.859305491403165</v>
       </c>
     </row>
     <row r="10">
@@ -3836,31 +3833,31 @@
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
       </c>
       <c r="E10" t="n">
-        <v>0.001962708537782139</v>
+        <v>0.4254170755642787</v>
       </c>
       <c r="F10" t="n">
         <v>0.7203140333660452</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2237487733071639</v>
+        <v>0.38763493621197254</v>
       </c>
       <c r="H10" t="n">
-        <v>0.02747791952894995</v>
+        <v>0.4342492639842983</v>
       </c>
       <c r="I10" t="n">
-        <v>0.016683022571148183</v>
+        <v>0.4278704612365064</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0</v>
+        <v>0.43866535819430813</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0</v>
+        <v>0.43719332679097156</v>
       </c>
       <c r="L10" t="n">
         <v>0.5602951702053611</v>
@@ -3928,7 +3925,7 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
         <v>41</v>
@@ -3937,22 +3934,22 @@
         <v>1.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.04072620215897939</v>
+        <v>0.41315014720314036</v>
       </c>
       <c r="G11" t="n">
         <v>0.9862610402355251</v>
       </c>
-      <c r="H11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>1.0</v>
+      <c r="H11" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" t="e">
+        <v>#DIV/0!</v>
       </c>
       <c r="K11" t="n">
-        <v>4.906771344455348E-4</v>
+        <v>0.42983316977428854</v>
       </c>
       <c r="L11" t="n">
         <v>0.5622018786890313</v>
@@ -4014,117 +4011,117 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
         <v>40</v>
       </c>
       <c r="E12" t="n">
-        <v>7.0</v>
+        <v>0.0030748206354629312</v>
       </c>
       <c r="F12" t="n">
-        <v>4.0</v>
+        <v>0.8390843867441066</v>
       </c>
       <c r="G12" t="n">
-        <v>7.0</v>
+        <v>0.5900239152716091</v>
       </c>
       <c r="H12" t="n">
-        <v>7.0</v>
+        <v>0.5497096002733174</v>
       </c>
       <c r="I12" t="n">
-        <v>7.0</v>
+        <v>0.8114110010249402</v>
       </c>
       <c r="J12" t="n">
-        <v>6.0</v>
+        <v>0.12401776563033823</v>
       </c>
       <c r="K12" t="n">
-        <v>6.0</v>
+        <v>0.15203279808677828</v>
       </c>
       <c r="L12" t="n">
-        <v>0.5602951702053611</v>
+        <v>0.9476657448856904</v>
       </c>
       <c r="M12" t="n">
-        <v>1.613898679837703</v>
+        <v>1.9791732004479081</v>
       </c>
       <c r="N12" t="n">
-        <v>5.327317965954149</v>
+        <v>0.0711034141514102</v>
       </c>
       <c r="O12" t="n">
-        <v>4.636286009871222</v>
+        <v>0.02572983671449778</v>
       </c>
       <c r="P12" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.397796817625459</v>
+        <v>0.17662951705504898</v>
       </c>
       <c r="R12" t="n">
-        <v>0.7258413264338339</v>
+        <v>0.9698014147633569</v>
       </c>
       <c r="S12" t="n">
-        <v>1634.0</v>
+        <v>2961.0</v>
       </c>
       <c r="T12" t="n">
-        <v>18158.0</v>
+        <v>20210.0</v>
       </c>
       <c r="U12" t="n">
-        <v>0.16718577785086547</v>
+        <v>0.8860374149599841</v>
       </c>
       <c r="V12" t="n">
-        <v>1.550027473303311</v>
+        <v>1.6408641369006336</v>
       </c>
       <c r="W12" t="n">
-        <v>17.805182288798328</v>
+        <v>0.06288965858485898</v>
       </c>
       <c r="X12" t="n">
-        <v>24.355242868157283</v>
+        <v>0.05390895596239485</v>
       </c>
       <c r="Y12" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.43473994111874387</v>
+        <v>0.4103177314656645</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.6653024736202267</v>
+        <v>0.9703252676415911</v>
       </c>
       <c r="AB12" t="n">
-        <v>2038.0</v>
+        <v>2927.0</v>
       </c>
       <c r="AC12" t="n">
-        <v>18158.0</v>
+        <v>20210.0</v>
       </c>
       <c r="AD12" t="n">
-        <v>260186.17743712067</v>
+        <v>768.936230306256</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
         <v>41</v>
       </c>
       <c r="E13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.4383327639221045</v>
+      </c>
+      <c r="G13" t="n">
         <v>1.0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>2.0</v>
       </c>
       <c r="H13" t="n">
         <v>1.0</v>
@@ -4136,167 +4133,167 @@
         <v>1.0</v>
       </c>
       <c r="K13" t="n">
-        <v>7.0</v>
+        <v>0.4229586607447899</v>
       </c>
       <c r="L13" t="n">
-        <v>0.5622018786890313</v>
+        <v>0.7370026973134763</v>
       </c>
       <c r="M13" t="n">
-        <v>1.613898679837703</v>
+        <v>1.9791732004479081</v>
       </c>
       <c r="N13" t="n">
-        <v>1.0003422257720689</v>
+        <v>0.999985053005148</v>
       </c>
       <c r="O13" t="n">
-        <v>6.017339481372286E-4</v>
+        <v>1.4301789093684736E-4</v>
       </c>
       <c r="P13" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.397796817625459</v>
+        <v>0.17662951705504898</v>
       </c>
       <c r="R13" t="n">
         <v>0.0</v>
       </c>
       <c r="S13" t="n">
-        <v>1634.0</v>
+        <v>2961.0</v>
       </c>
       <c r="T13" t="n">
-        <v>8755.0</v>
+        <v>9179.0</v>
       </c>
       <c r="U13" t="n">
-        <v>0.6023658796459858</v>
+        <v>0.7842590352584322</v>
       </c>
       <c r="V13" t="n">
-        <v>1.550027473303311</v>
+        <v>1.6408641369006336</v>
       </c>
       <c r="W13" t="n">
-        <v>1.0004491461137193</v>
+        <v>0.9999805334118116</v>
       </c>
       <c r="X13" t="n">
-        <v>6.064841273867305E-4</v>
+        <v>1.4056114320615265E-4</v>
       </c>
       <c r="Y13" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.43473994111874387</v>
+        <v>0.4103177314656645</v>
       </c>
       <c r="AA13" t="n">
         <v>0.0</v>
       </c>
       <c r="AB13" t="n">
-        <v>2038.0</v>
+        <v>2927.0</v>
       </c>
       <c r="AC13" t="n">
-        <v>8755.0</v>
+        <v>9179.0</v>
       </c>
       <c r="AD13" t="n">
-        <v>3.859305491403165</v>
+        <v>2.0968871659786887</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
       </c>
       <c r="E14" t="n">
-        <v>0.4254170755642787</v>
+        <v>0.33071404168090196</v>
       </c>
       <c r="F14" t="n">
-        <v>0.7203140333660452</v>
+        <v>0.8390843867441066</v>
       </c>
       <c r="G14" t="n">
-        <v>0.38763493621197254</v>
+        <v>0.5900239152716091</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4342492639842983</v>
+        <v>0.5497096002733174</v>
       </c>
       <c r="I14" t="n">
-        <v>0.4278704612365064</v>
+        <v>0.8114110010249402</v>
       </c>
       <c r="J14" t="n">
-        <v>0.43866535819430813</v>
+        <v>0.299624188588999</v>
       </c>
       <c r="K14" t="n">
-        <v>0.43719332679097156</v>
+        <v>0.39050222070379226</v>
       </c>
       <c r="L14" t="n">
-        <v>0.5602951702053611</v>
+        <v>0.9476657448856904</v>
       </c>
       <c r="M14" t="n">
-        <v>1.613898679837703</v>
+        <v>1.9791732004479081</v>
       </c>
       <c r="N14" t="n">
-        <v>5.327317965954149</v>
+        <v>0.0711034141514102</v>
       </c>
       <c r="O14" t="n">
-        <v>4.636286009871222</v>
+        <v>0.02572983671449778</v>
       </c>
       <c r="P14" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.397796817625459</v>
+        <v>0.17662951705504898</v>
       </c>
       <c r="R14" t="n">
-        <v>0.7258413264338339</v>
+        <v>0.9698014147633569</v>
       </c>
       <c r="S14" t="n">
-        <v>1634.0</v>
+        <v>2961.0</v>
       </c>
       <c r="T14" t="n">
-        <v>18158.0</v>
+        <v>20210.0</v>
       </c>
       <c r="U14" t="n">
-        <v>0.16718577785086547</v>
+        <v>0.8860374149599841</v>
       </c>
       <c r="V14" t="n">
-        <v>1.550027473303311</v>
+        <v>1.6408641369006336</v>
       </c>
       <c r="W14" t="n">
-        <v>17.805182288798328</v>
+        <v>0.06288965858485898</v>
       </c>
       <c r="X14" t="n">
-        <v>24.355242868157283</v>
+        <v>0.05390895596239485</v>
       </c>
       <c r="Y14" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.43473994111874387</v>
+        <v>0.4103177314656645</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.6653024736202267</v>
+        <v>0.9703252676415911</v>
       </c>
       <c r="AB14" t="n">
-        <v>2038.0</v>
+        <v>2927.0</v>
       </c>
       <c r="AC14" t="n">
-        <v>18158.0</v>
+        <v>20210.0</v>
       </c>
       <c r="AD14" t="n">
-        <v>260186.17743712067</v>
+        <v>768.936230306256</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
         <v>41</v>
@@ -4305,10 +4302,10 @@
         <v>1.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.41315014720314036</v>
+        <v>0.4383327639221045</v>
       </c>
       <c r="G15" t="n">
-        <v>0.9862610402355251</v>
+        <v>1.0</v>
       </c>
       <c r="H15" t="e">
         <v>#DIV/0!</v>
@@ -4320,72 +4317,72 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K15" t="n">
-        <v>0.42983316977428854</v>
+        <v>0.4229586607447899</v>
       </c>
       <c r="L15" t="n">
-        <v>0.5622018786890313</v>
+        <v>0.7370026973134763</v>
       </c>
       <c r="M15" t="n">
-        <v>1.613898679837703</v>
+        <v>1.9791732004479081</v>
       </c>
       <c r="N15" t="n">
-        <v>1.0003422257720689</v>
+        <v>0.999985053005148</v>
       </c>
       <c r="O15" t="n">
-        <v>6.017339481372286E-4</v>
+        <v>1.4301789093684736E-4</v>
       </c>
       <c r="P15" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.397796817625459</v>
+        <v>0.17662951705504898</v>
       </c>
       <c r="R15" t="n">
         <v>0.0</v>
       </c>
       <c r="S15" t="n">
-        <v>1634.0</v>
+        <v>2961.0</v>
       </c>
       <c r="T15" t="n">
-        <v>8755.0</v>
+        <v>9179.0</v>
       </c>
       <c r="U15" t="n">
-        <v>0.6023658796459858</v>
+        <v>0.7842590352584322</v>
       </c>
       <c r="V15" t="n">
-        <v>1.550027473303311</v>
+        <v>1.6408641369006336</v>
       </c>
       <c r="W15" t="n">
-        <v>1.0004491461137193</v>
+        <v>0.9999805334118116</v>
       </c>
       <c r="X15" t="n">
-        <v>6.064841273867305E-4</v>
+        <v>1.4056114320615265E-4</v>
       </c>
       <c r="Y15" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.43473994111874387</v>
+        <v>0.4103177314656645</v>
       </c>
       <c r="AA15" t="n">
         <v>0.0</v>
       </c>
       <c r="AB15" t="n">
-        <v>2038.0</v>
+        <v>2927.0</v>
       </c>
       <c r="AC15" t="n">
-        <v>8755.0</v>
+        <v>9179.0</v>
       </c>
       <c r="AD15" t="n">
-        <v>3.859305491403165</v>
+        <v>2.0968871659786887</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>46</v>
@@ -4394,90 +4391,90 @@
         <v>40</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0030748206354629312</v>
+        <v>0.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8390843867441066</v>
+        <v>0.09759686120647376</v>
       </c>
       <c r="G16" t="n">
-        <v>0.5900239152716091</v>
+        <v>0.3545855811672388</v>
       </c>
       <c r="H16" t="n">
-        <v>0.5497096002733174</v>
+        <v>0.02893575282000981</v>
       </c>
       <c r="I16" t="n">
-        <v>0.8114110010249402</v>
+        <v>0.05934281510544385</v>
       </c>
       <c r="J16" t="n">
-        <v>0.12401776563033823</v>
+        <v>0.024031387935262383</v>
       </c>
       <c r="K16" t="n">
-        <v>0.15203279808677828</v>
+        <v>0.0</v>
       </c>
       <c r="L16" t="n">
-        <v>0.9476657448856904</v>
+        <v>0.1649256844160517</v>
       </c>
       <c r="M16" t="n">
-        <v>1.9791732004479081</v>
+        <v>1.5507979694968936</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0711034141514102</v>
+        <v>17.67925884955752</v>
       </c>
       <c r="O16" t="n">
-        <v>0.02572983671449778</v>
+        <v>23.639518805309734</v>
       </c>
       <c r="P16" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.17662951705504898</v>
+        <v>0.43443627450980393</v>
       </c>
       <c r="R16" t="n">
-        <v>0.9698014147633569</v>
+        <v>0.6634832050906646</v>
       </c>
       <c r="S16" t="n">
-        <v>2961.0</v>
+        <v>1632.0</v>
       </c>
       <c r="T16" t="n">
-        <v>20210.0</v>
+        <v>18080.0</v>
       </c>
       <c r="U16" t="n">
-        <v>0.8860374149599841</v>
+        <v>0.5557317440586943</v>
       </c>
       <c r="V16" t="n">
-        <v>1.6408641369006336</v>
+        <v>1.612996543699384</v>
       </c>
       <c r="W16" t="n">
-        <v>0.06288965858485898</v>
+        <v>5.359897649164202</v>
       </c>
       <c r="X16" t="n">
-        <v>0.05390895596239485</v>
+        <v>4.721558445301237</v>
       </c>
       <c r="Y16" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.4103177314656645</v>
+        <v>0.39823442864149095</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.9703252676415911</v>
+        <v>0.7241158037733229</v>
       </c>
       <c r="AB16" t="n">
-        <v>2927.0</v>
+        <v>2039.0</v>
       </c>
       <c r="AC16" t="n">
-        <v>20210.0</v>
+        <v>18080.0</v>
       </c>
       <c r="AD16" t="n">
-        <v>768.936230306256</v>
+        <v>253790.21565370838</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>46</v>
@@ -4489,10 +4486,10 @@
         <v>0.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.4383327639221045</v>
+        <v>0.06817067189798921</v>
       </c>
       <c r="G17" t="n">
-        <v>1.0</v>
+        <v>0.9597842079450711</v>
       </c>
       <c r="H17" t="n">
         <v>1.0</v>
@@ -4504,72 +4501,72 @@
         <v>1.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.4229586607447899</v>
+        <v>0.0</v>
       </c>
       <c r="L17" t="n">
-        <v>0.7370026973134763</v>
+        <v>0.5937233143793375</v>
       </c>
       <c r="M17" t="n">
-        <v>1.9791732004479081</v>
+        <v>1.5507979694968936</v>
       </c>
       <c r="N17" t="n">
-        <v>0.999985053005148</v>
+        <v>1.000695557113135</v>
       </c>
       <c r="O17" t="n">
-        <v>1.4301789093684736E-4</v>
+        <v>8.479671646970388E-4</v>
       </c>
       <c r="P17" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.17662951705504898</v>
+        <v>0.43443627450980393</v>
       </c>
       <c r="R17" t="n">
         <v>0.0</v>
       </c>
       <c r="S17" t="n">
-        <v>2961.0</v>
+        <v>1632.0</v>
       </c>
       <c r="T17" t="n">
-        <v>9179.0</v>
+        <v>8705.0</v>
       </c>
       <c r="U17" t="n">
-        <v>0.7842590352584322</v>
+        <v>0.5798576193243599</v>
       </c>
       <c r="V17" t="n">
-        <v>1.6408641369006336</v>
+        <v>1.612996543699384</v>
       </c>
       <c r="W17" t="n">
-        <v>0.9999805334118116</v>
+        <v>1.0003840948212157</v>
       </c>
       <c r="X17" t="n">
-        <v>1.4056114320615265E-4</v>
+        <v>8.296245648722333E-4</v>
       </c>
       <c r="Y17" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.4103177314656645</v>
+        <v>0.39823442864149095</v>
       </c>
       <c r="AA17" t="n">
         <v>0.0</v>
       </c>
       <c r="AB17" t="n">
-        <v>2927.0</v>
+        <v>2039.0</v>
       </c>
       <c r="AC17" t="n">
-        <v>9179.0</v>
+        <v>8705.0</v>
       </c>
       <c r="AD17" t="n">
-        <v>2.0968871659786887</v>
+        <v>5.042908715055177</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
@@ -4578,90 +4575,90 @@
         <v>40</v>
       </c>
       <c r="E18" t="n">
-        <v>8.0</v>
+        <v>0.38695438940657184</v>
       </c>
       <c r="F18" t="n">
-        <v>5.0</v>
+        <v>0.3712604217753801</v>
       </c>
       <c r="G18" t="n">
+        <v>0.3545855811672388</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.38940657184894556</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.3820500245218244</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.39382050024521825</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.3987248651299657</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.1649256844160517</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1.5507979694968936</v>
+      </c>
+      <c r="N18" t="n">
+        <v>17.67925884955752</v>
+      </c>
+      <c r="O18" t="n">
+        <v>23.639518805309734</v>
+      </c>
+      <c r="P18" t="n">
         <v>6.0</v>
       </c>
-      <c r="H18" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="J18" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="K18" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.9476657448856904</v>
-      </c>
-      <c r="M18" t="n">
-        <v>1.9791732004479081</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0.0711034141514102</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0.02572983671449778</v>
-      </c>
-      <c r="P18" t="n">
-        <v>8.0</v>
-      </c>
       <c r="Q18" t="n">
-        <v>0.17662951705504898</v>
+        <v>0.43443627450980393</v>
       </c>
       <c r="R18" t="n">
-        <v>0.9698014147633569</v>
+        <v>0.6634832050906646</v>
       </c>
       <c r="S18" t="n">
-        <v>2961.0</v>
+        <v>1632.0</v>
       </c>
       <c r="T18" t="n">
-        <v>20210.0</v>
+        <v>18080.0</v>
       </c>
       <c r="U18" t="n">
-        <v>0.8860374149599841</v>
+        <v>0.5557317440586943</v>
       </c>
       <c r="V18" t="n">
-        <v>1.6408641369006336</v>
+        <v>1.612996543699384</v>
       </c>
       <c r="W18" t="n">
-        <v>0.06288965858485898</v>
+        <v>5.359897649164202</v>
       </c>
       <c r="X18" t="n">
-        <v>0.05390895596239485</v>
+        <v>4.721558445301237</v>
       </c>
       <c r="Y18" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.4103177314656645</v>
+        <v>0.39823442864149095</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.9703252676415911</v>
+        <v>0.7241158037733229</v>
       </c>
       <c r="AB18" t="n">
-        <v>2927.0</v>
+        <v>2039.0</v>
       </c>
       <c r="AC18" t="n">
-        <v>20210.0</v>
+        <v>18080.0</v>
       </c>
       <c r="AD18" t="n">
-        <v>768.936230306256</v>
+        <v>253790.21565370838</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
         <v>47</v>
@@ -4673,814 +4670,78 @@
         <v>1.0</v>
       </c>
       <c r="F19" t="n">
+        <v>0.3830308974987739</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.9597842079450711</v>
+      </c>
+      <c r="H19" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J19" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.3874448258950466</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.5937233143793375</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1.5507979694968936</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1.000695557113135</v>
+      </c>
+      <c r="O19" t="n">
+        <v>8.479671646970388E-4</v>
+      </c>
+      <c r="P19" t="n">
         <v>6.0</v>
       </c>
-      <c r="G19" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H19" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I19" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J19" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="K19" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0.7370026973134763</v>
-      </c>
-      <c r="M19" t="n">
-        <v>1.9791732004479081</v>
-      </c>
-      <c r="N19" t="n">
-        <v>0.999985053005148</v>
-      </c>
-      <c r="O19" t="n">
-        <v>1.4301789093684736E-4</v>
-      </c>
-      <c r="P19" t="n">
-        <v>8.0</v>
-      </c>
       <c r="Q19" t="n">
-        <v>0.17662951705504898</v>
+        <v>0.43443627450980393</v>
       </c>
       <c r="R19" t="n">
         <v>0.0</v>
       </c>
       <c r="S19" t="n">
-        <v>2961.0</v>
+        <v>1632.0</v>
       </c>
       <c r="T19" t="n">
-        <v>9179.0</v>
+        <v>8705.0</v>
       </c>
       <c r="U19" t="n">
-        <v>0.7842590352584322</v>
+        <v>0.5798576193243599</v>
       </c>
       <c r="V19" t="n">
-        <v>1.6408641369006336</v>
+        <v>1.612996543699384</v>
       </c>
       <c r="W19" t="n">
-        <v>0.9999805334118116</v>
+        <v>1.0003840948212157</v>
       </c>
       <c r="X19" t="n">
-        <v>1.4056114320615265E-4</v>
+        <v>8.296245648722333E-4</v>
       </c>
       <c r="Y19" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.4103177314656645</v>
+        <v>0.39823442864149095</v>
       </c>
       <c r="AA19" t="n">
         <v>0.0</v>
       </c>
       <c r="AB19" t="n">
-        <v>2927.0</v>
+        <v>2039.0</v>
       </c>
       <c r="AC19" t="n">
-        <v>9179.0</v>
+        <v>8705.0</v>
       </c>
       <c r="AD19" t="n">
-        <v>2.0968871659786887</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.33071404168090196</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.8390843867441066</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.5900239152716091</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.5497096002733174</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0.8114110010249402</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0.299624188588999</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0.39050222070379226</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0.9476657448856904</v>
-      </c>
-      <c r="M20" t="n">
-        <v>1.9791732004479081</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0.0711034141514102</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0.02572983671449778</v>
-      </c>
-      <c r="P20" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>0.17662951705504898</v>
-      </c>
-      <c r="R20" t="n">
-        <v>0.9698014147633569</v>
-      </c>
-      <c r="S20" t="n">
-        <v>2961.0</v>
-      </c>
-      <c r="T20" t="n">
-        <v>20210.0</v>
-      </c>
-      <c r="U20" t="n">
-        <v>0.8860374149599841</v>
-      </c>
-      <c r="V20" t="n">
-        <v>1.6408641369006336</v>
-      </c>
-      <c r="W20" t="n">
-        <v>0.06288965858485898</v>
-      </c>
-      <c r="X20" t="n">
-        <v>0.05390895596239485</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>0.4103177314656645</v>
-      </c>
-      <c r="AA20" t="n">
-        <v>0.9703252676415911</v>
-      </c>
-      <c r="AB20" t="n">
-        <v>2927.0</v>
-      </c>
-      <c r="AC20" t="n">
-        <v>20210.0</v>
-      </c>
-      <c r="AD20" t="n">
-        <v>768.936230306256</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.4383327639221045</v>
-      </c>
-      <c r="G21" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="H21" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J21" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0.4229586607447899</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0.7370026973134763</v>
-      </c>
-      <c r="M21" t="n">
-        <v>1.9791732004479081</v>
-      </c>
-      <c r="N21" t="n">
-        <v>0.999985053005148</v>
-      </c>
-      <c r="O21" t="n">
-        <v>1.4301789093684736E-4</v>
-      </c>
-      <c r="P21" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>0.17662951705504898</v>
-      </c>
-      <c r="R21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S21" t="n">
-        <v>2961.0</v>
-      </c>
-      <c r="T21" t="n">
-        <v>9179.0</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0.7842590352584322</v>
-      </c>
-      <c r="V21" t="n">
-        <v>1.6408641369006336</v>
-      </c>
-      <c r="W21" t="n">
-        <v>0.9999805334118116</v>
-      </c>
-      <c r="X21" t="n">
-        <v>1.4056114320615265E-4</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>0.4103177314656645</v>
-      </c>
-      <c r="AA21" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AB21" t="n">
-        <v>2927.0</v>
-      </c>
-      <c r="AC21" t="n">
-        <v>9179.0</v>
-      </c>
-      <c r="AD21" t="n">
-        <v>2.0968871659786887</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.09759686120647376</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.3545855811672388</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.02893575282000981</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.05934281510544385</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0.024031387935262383</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0.1649256844160517</v>
-      </c>
-      <c r="M22" t="n">
-        <v>1.5507979694968936</v>
-      </c>
-      <c r="N22" t="n">
-        <v>17.67925884955752</v>
-      </c>
-      <c r="O22" t="n">
-        <v>23.639518805309734</v>
-      </c>
-      <c r="P22" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0.43443627450980393</v>
-      </c>
-      <c r="R22" t="n">
-        <v>0.6634832050906646</v>
-      </c>
-      <c r="S22" t="n">
-        <v>1632.0</v>
-      </c>
-      <c r="T22" t="n">
-        <v>18080.0</v>
-      </c>
-      <c r="U22" t="n">
-        <v>0.5557317440586943</v>
-      </c>
-      <c r="V22" t="n">
-        <v>1.612996543699384</v>
-      </c>
-      <c r="W22" t="n">
-        <v>5.359897649164202</v>
-      </c>
-      <c r="X22" t="n">
-        <v>4.721558445301237</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="Z22" t="n">
-        <v>0.39823442864149095</v>
-      </c>
-      <c r="AA22" t="n">
-        <v>0.7241158037733229</v>
-      </c>
-      <c r="AB22" t="n">
-        <v>2039.0</v>
-      </c>
-      <c r="AC22" t="n">
-        <v>18080.0</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>253790.21565370838</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.06817067189798921</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.9597842079450711</v>
-      </c>
-      <c r="H23" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I23" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J23" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0.5937233143793375</v>
-      </c>
-      <c r="M23" t="n">
-        <v>1.5507979694968936</v>
-      </c>
-      <c r="N23" t="n">
-        <v>1.000695557113135</v>
-      </c>
-      <c r="O23" t="n">
-        <v>8.479671646970388E-4</v>
-      </c>
-      <c r="P23" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0.43443627450980393</v>
-      </c>
-      <c r="R23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S23" t="n">
-        <v>1632.0</v>
-      </c>
-      <c r="T23" t="n">
-        <v>8705.0</v>
-      </c>
-      <c r="U23" t="n">
-        <v>0.5798576193243599</v>
-      </c>
-      <c r="V23" t="n">
-        <v>1.612996543699384</v>
-      </c>
-      <c r="W23" t="n">
-        <v>1.0003840948212157</v>
-      </c>
-      <c r="X23" t="n">
-        <v>8.296245648722333E-4</v>
-      </c>
-      <c r="Y23" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="Z23" t="n">
-        <v>0.39823442864149095</v>
-      </c>
-      <c r="AA23" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AB23" t="n">
-        <v>2039.0</v>
-      </c>
-      <c r="AC23" t="n">
-        <v>8705.0</v>
-      </c>
-      <c r="AD23" t="n">
-        <v>5.042908715055177</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="H24" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="I24" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="J24" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="K24" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0.1649256844160517</v>
-      </c>
-      <c r="M24" t="n">
-        <v>1.5507979694968936</v>
-      </c>
-      <c r="N24" t="n">
-        <v>17.67925884955752</v>
-      </c>
-      <c r="O24" t="n">
-        <v>23.639518805309734</v>
-      </c>
-      <c r="P24" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0.43443627450980393</v>
-      </c>
-      <c r="R24" t="n">
-        <v>0.6634832050906646</v>
-      </c>
-      <c r="S24" t="n">
-        <v>1632.0</v>
-      </c>
-      <c r="T24" t="n">
-        <v>18080.0</v>
-      </c>
-      <c r="U24" t="n">
-        <v>0.5557317440586943</v>
-      </c>
-      <c r="V24" t="n">
-        <v>1.612996543699384</v>
-      </c>
-      <c r="W24" t="n">
-        <v>5.359897649164202</v>
-      </c>
-      <c r="X24" t="n">
-        <v>4.721558445301237</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>0.39823442864149095</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>0.7241158037733229</v>
-      </c>
-      <c r="AB24" t="n">
-        <v>2039.0</v>
-      </c>
-      <c r="AC24" t="n">
-        <v>18080.0</v>
-      </c>
-      <c r="AD24" t="n">
-        <v>253790.21565370838</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="H25" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I25" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0.5937233143793375</v>
-      </c>
-      <c r="M25" t="n">
-        <v>1.5507979694968936</v>
-      </c>
-      <c r="N25" t="n">
-        <v>1.000695557113135</v>
-      </c>
-      <c r="O25" t="n">
-        <v>8.479671646970388E-4</v>
-      </c>
-      <c r="P25" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>0.43443627450980393</v>
-      </c>
-      <c r="R25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S25" t="n">
-        <v>1632.0</v>
-      </c>
-      <c r="T25" t="n">
-        <v>8705.0</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0.5798576193243599</v>
-      </c>
-      <c r="V25" t="n">
-        <v>1.612996543699384</v>
-      </c>
-      <c r="W25" t="n">
-        <v>1.0003840948212157</v>
-      </c>
-      <c r="X25" t="n">
-        <v>8.296245648722333E-4</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>0.39823442864149095</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AB25" t="n">
-        <v>2039.0</v>
-      </c>
-      <c r="AC25" t="n">
-        <v>8705.0</v>
-      </c>
-      <c r="AD25" t="n">
-        <v>5.042908715055177</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.38695438940657184</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.3712604217753801</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.3545855811672388</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.38940657184894556</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0.3820500245218244</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0.39382050024521825</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0.3987248651299657</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0.1649256844160517</v>
-      </c>
-      <c r="M26" t="n">
-        <v>1.5507979694968936</v>
-      </c>
-      <c r="N26" t="n">
-        <v>17.67925884955752</v>
-      </c>
-      <c r="O26" t="n">
-        <v>23.639518805309734</v>
-      </c>
-      <c r="P26" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>0.43443627450980393</v>
-      </c>
-      <c r="R26" t="n">
-        <v>0.6634832050906646</v>
-      </c>
-      <c r="S26" t="n">
-        <v>1632.0</v>
-      </c>
-      <c r="T26" t="n">
-        <v>18080.0</v>
-      </c>
-      <c r="U26" t="n">
-        <v>0.5557317440586943</v>
-      </c>
-      <c r="V26" t="n">
-        <v>1.612996543699384</v>
-      </c>
-      <c r="W26" t="n">
-        <v>5.359897649164202</v>
-      </c>
-      <c r="X26" t="n">
-        <v>4.721558445301237</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="Z26" t="n">
-        <v>0.39823442864149095</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>0.7241158037733229</v>
-      </c>
-      <c r="AB26" t="n">
-        <v>2039.0</v>
-      </c>
-      <c r="AC26" t="n">
-        <v>18080.0</v>
-      </c>
-      <c r="AD26" t="n">
-        <v>253790.21565370838</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0.3830308974987739</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.9597842079450711</v>
-      </c>
-      <c r="H27" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I27" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J27" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0.3874448258950466</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0.5937233143793375</v>
-      </c>
-      <c r="M27" t="n">
-        <v>1.5507979694968936</v>
-      </c>
-      <c r="N27" t="n">
-        <v>1.000695557113135</v>
-      </c>
-      <c r="O27" t="n">
-        <v>8.479671646970388E-4</v>
-      </c>
-      <c r="P27" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="Q27" t="n">
-        <v>0.43443627450980393</v>
-      </c>
-      <c r="R27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="S27" t="n">
-        <v>1632.0</v>
-      </c>
-      <c r="T27" t="n">
-        <v>8705.0</v>
-      </c>
-      <c r="U27" t="n">
-        <v>0.5798576193243599</v>
-      </c>
-      <c r="V27" t="n">
-        <v>1.612996543699384</v>
-      </c>
-      <c r="W27" t="n">
-        <v>1.0003840948212157</v>
-      </c>
-      <c r="X27" t="n">
-        <v>8.296245648722333E-4</v>
-      </c>
-      <c r="Y27" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="Z27" t="n">
-        <v>0.39823442864149095</v>
-      </c>
-      <c r="AA27" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AB27" t="n">
-        <v>2039.0</v>
-      </c>
-      <c r="AC27" t="n">
-        <v>8705.0</v>
-      </c>
-      <c r="AD27" t="n">
         <v>5.042908715055177</v>
       </c>
     </row>

</xml_diff>